<commit_message>
i229--EIT2 ta suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/analysis_00_ta_engine_all.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/analysis_00_ta_engine_all.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\new_eit2\eit2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\test\analysis_00_ta_engine\hold_correction\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="DD9F" lockStructure="1"/>
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1050" activeSheetId="2"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1050" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="437">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -993,10 +993,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>cmd = python DEV/bin/run_diamondng.py --devkit=iCE40UP5K-CM225I --synthesis=lse  --run-par-trce</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>repository = http://lshlabd0011/radiant/trunk/general</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1512,9 +1508,6 @@
     <t>create_generated_clock</t>
   </si>
   <si>
-    <t>SDC_cases/02_create_generated_clock/edges_nets_01</t>
-  </si>
-  <si>
     <t>SDC_cases/10_set_false_path/to_cells_01</t>
   </si>
   <si>
@@ -1523,13 +1516,74 @@
   </si>
   <si>
     <t>radiant=ng1_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDC_cases/02_create_generated_clock/edges_nets_01</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">IO Timing </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDC_cases/14_new_feature/IO_timing/case</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>83</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold correction</t>
+  </si>
+  <si>
+    <t>hold correction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold correction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>84</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold_correction/hold_correction1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold_correction/hold_correction2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold_correction/hold_correction3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd = python DEV/bin/run_diamondng.py  --synthesis=lse  --run-par-iota</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2726,9 +2780,37 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2741,9 +2823,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2757,31 +2836,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5189,71 +5243,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{00286210-A62E-4369-B184-F0CCBF626B73}" diskRevisions="1" revisionId="1349" version="31">
-  <header guid="{9662F072-F305-4FFD-BA13-D3D8485EDFAC}" dateTime="2018-10-11T16:49:08" maxSheetId="5" userName="Jason Wang" r:id="rId21" minRId="1329" maxRId="1331">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DA349982-2D27-4384-AC61-72AEC3CFAC9B}" dateTime="2018-10-11T16:49:20" maxSheetId="5" userName="Jason Wang" r:id="rId22">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F06636B5-9DA9-4C3B-BE97-339A38155DCE}" dateTime="2018-10-11T16:49:52" maxSheetId="5" userName="Jason Wang" r:id="rId23" minRId="1332">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{223153B4-09DC-4EB8-A14F-3470A5F2E012}" dateTime="2018-10-11T16:50:00" maxSheetId="5" userName="Jason Wang" r:id="rId24" minRId="1334" maxRId="1335">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1BB109A1-A8E5-4466-AB6B-1D64F9666CDA}" dateTime="2018-10-11T16:50:59" maxSheetId="5" userName="Jason Wang" r:id="rId25" minRId="1337" maxRId="1342">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{2BA1918A-761E-427C-87DD-7D4068FB9A30}" dateTime="2018-10-11T16:51:01" maxSheetId="5" userName="Jason Wang" r:id="rId26">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{81461A94-5291-4B85-AB9B-D4B859964E32}" dateTime="2018-10-12T11:00:00" maxSheetId="5" userName="Jason Wang" r:id="rId27" minRId="1345">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{2E8DC6AD-3446-44C0-BCE1-EC15014537E2}" dateTime="2018-10-12T11:01:32" maxSheetId="5" userName="Jason Wang" r:id="rId28" minRId="1346">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{655D6220-6132-41C2-8290-FCF487860342}" diskRevisions="1" revisionId="1450" version="35">
   <header guid="{962A471B-F009-4B00-939D-E8F2DC59916E}" dateTime="2018-10-12T14:54:08" maxSheetId="5" userName="Jason Wang" r:id="rId29" minRId="1347">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5278,87 +5268,104 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{4F49597B-E632-4416-AC35-916C5363D7A3}" dateTime="2019-10-23T11:24:21" maxSheetId="5" userName="Jason Wang" r:id="rId32" minRId="1350" maxRId="1356">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4DF6F27E-B6DD-4B21-BBD6-D13DECFDE97C}" dateTime="2019-10-23T11:25:53" maxSheetId="5" userName="Jason Wang" r:id="rId33" minRId="1357" maxRId="1446">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{85564795-2032-474C-BD9F-D834A0FAC29D}" dateTime="2019-10-23T11:26:14" maxSheetId="5" userName="Jason Wang" r:id="rId34" minRId="1448">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{655D6220-6132-41C2-8290-FCF487860342}" dateTime="2019-10-23T11:27:12" maxSheetId="5" userName="Jason Wang" r:id="rId35">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1329" sId="2" odxf="1" dxf="1">
-    <nc r="D82" t="inlineStr">
-      <is>
-        <t>set_clock_uncertainty</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
+  <rcc rId="1350" sId="2">
+    <oc r="E84" t="inlineStr">
+      <is>
+        <t>SDC_cases/02_create_generated_clock/edges_nets_01</t>
+      </is>
+    </oc>
+    <nc r="E84" t="inlineStr">
+      <is>
+        <t>SDC_cases/02_create_generated_clock/edges_nets_01</t>
+        <phoneticPr fontId="0" type="noConversion"/>
       </is>
     </nc>
-    <odxf>
+  </rcc>
+  <rcc rId="1351" sId="2">
+    <nc r="D85" t="inlineStr">
+      <is>
+        <t xml:space="preserve">IO Timing </t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1352" sId="2">
+    <nc r="E85" t="inlineStr">
+      <is>
+        <t>SDC_cases/14_new_feature/IO_timing/case</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1353" sId="2">
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>83</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1354" sId="2">
+    <nc r="D86" t="inlineStr">
+      <is>
+        <t>hold correction</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1355" sId="2" xfDxf="1" dxf="1">
+    <nc r="D87" t="inlineStr">
+      <is>
+        <t>hold correction</t>
+      </is>
+    </nc>
+    <ndxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="bottom" readingOrder="0"/>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <protection locked="0"/>
     </ndxf>
   </rcc>
-  <rcc rId="1330" sId="2" odxf="1" dxf="1">
-    <nc r="E82" t="inlineStr">
-      <is>
-        <t>SDC_cases/04_set_clock_uncertainty/from_to_02</t>
-      </is>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="bottom" readingOrder="0"/>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="1331" sId="2">
-    <nc r="A82" t="inlineStr">
-      <is>
-        <t>80</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
+  <rcc rId="1356" sId="2">
+    <nc r="D88" t="inlineStr">
+      <is>
+        <t>hold correction</t>
+        <phoneticPr fontId="0" type="noConversion"/>
       </is>
     </nc>
   </rcc>
@@ -5404,40 +5411,752 @@
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="D82" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="bottom" readingOrder="0"/>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="E82" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="bottom" readingOrder="0"/>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-  </rfmt>
+  <rcc rId="1357" sId="2">
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1358" sId="2">
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1359" sId="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_diamondng.py --devkit=iCE40UP5K-CM225I --synthesis=lse  --run-par-trce</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_diamondng.py  --synthesis=lse  --run-par-trce</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1360" sId="2">
+    <nc r="M3" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1361" sId="2">
+    <nc r="M4" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1362" sId="2">
+    <nc r="M5" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1363" sId="2">
+    <nc r="M6" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1364" sId="2">
+    <nc r="M7" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1365" sId="2">
+    <nc r="M8" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1366" sId="2">
+    <nc r="M9" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1367" sId="2">
+    <nc r="M10" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1368" sId="2">
+    <nc r="M11" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1369" sId="2">
+    <nc r="M12" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1370" sId="2">
+    <nc r="M13" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1371" sId="2">
+    <nc r="M14" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1372" sId="2">
+    <nc r="M15" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1373" sId="2">
+    <nc r="M16" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1374" sId="2">
+    <nc r="M17" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1375" sId="2">
+    <nc r="M18" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1376" sId="2">
+    <nc r="M19" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1377" sId="2">
+    <nc r="M20" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1378" sId="2">
+    <nc r="M21" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1379" sId="2">
+    <nc r="M22" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1380" sId="2">
+    <nc r="M23" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1381" sId="2">
+    <nc r="M24" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1382" sId="2">
+    <nc r="M25" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1383" sId="2">
+    <nc r="M26" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1384" sId="2">
+    <nc r="M27" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1385" sId="2">
+    <nc r="M28" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1386" sId="2">
+    <nc r="M29" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1387" sId="2">
+    <nc r="M30" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1388" sId="2">
+    <nc r="M31" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1389" sId="2">
+    <nc r="M32" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1390" sId="2">
+    <nc r="M33" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1391" sId="2">
+    <nc r="M34" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1392" sId="2">
+    <nc r="M35" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1393" sId="2">
+    <nc r="M36" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1394" sId="2">
+    <nc r="M37" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1395" sId="2">
+    <nc r="M38" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1396" sId="2">
+    <nc r="M39" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1397" sId="2">
+    <nc r="M40" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1398" sId="2">
+    <nc r="M41" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1399" sId="2">
+    <nc r="M42" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1400" sId="2">
+    <nc r="M43" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1401" sId="2">
+    <nc r="M44" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1402" sId="2">
+    <nc r="M45" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1403" sId="2">
+    <nc r="M46" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1404" sId="2">
+    <nc r="M47" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1405" sId="2">
+    <nc r="M48" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1406" sId="2">
+    <nc r="M49" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1407" sId="2">
+    <nc r="M50" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1408" sId="2">
+    <nc r="M51" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1409" sId="2">
+    <nc r="M52" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1410" sId="2">
+    <nc r="M53" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1411" sId="2">
+    <nc r="M54" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1412" sId="2">
+    <nc r="M55" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1413" sId="2">
+    <nc r="M56" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1414" sId="2">
+    <nc r="M57" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1415" sId="2">
+    <nc r="M58" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1416" sId="2">
+    <nc r="M59" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1417" sId="2">
+    <nc r="M60" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1418" sId="2">
+    <nc r="M61" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1419" sId="2">
+    <nc r="M62" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1420" sId="2">
+    <nc r="M63" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1421" sId="2">
+    <nc r="M64" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1422" sId="2">
+    <nc r="M65" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1423" sId="2">
+    <nc r="M66" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1424" sId="2">
+    <nc r="M67" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1425" sId="2">
+    <nc r="M68" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1426" sId="2">
+    <nc r="M69" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1427" sId="2">
+    <nc r="M70" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1428" sId="2">
+    <nc r="M71" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1429" sId="2">
+    <nc r="M72" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1430" sId="2">
+    <nc r="M73" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1431" sId="2">
+    <nc r="M74" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1432" sId="2">
+    <nc r="M75" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1433" sId="2">
+    <nc r="M76" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1434" sId="2">
+    <nc r="M77" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1435" sId="2">
+    <nc r="M78" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1436" sId="2">
+    <nc r="M79" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1437" sId="2">
+    <nc r="M80" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1438" sId="2">
+    <nc r="M81" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1439" sId="2">
+    <nc r="M82" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1440" sId="2">
+    <nc r="M83" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1441" sId="2">
+    <nc r="M84" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1442" sId="2">
+    <nc r="M85" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1443" sId="2">
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>84</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1444" sId="2">
+    <nc r="E86" t="inlineStr">
+      <is>
+        <t>hold_correction/hold_correction1</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1445" sId="2">
+    <nc r="E87" t="inlineStr">
+      <is>
+        <t>hold_correction/hold_correction2</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1446" sId="2">
+    <nc r="E88" t="inlineStr">
+      <is>
+        <t>hold_correction/hold_correction3</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AB$2</formula>
+    <oldFormula>case!$A$2:$AB$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
 </revisions>
 </file>
 
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1332" sId="2">
-    <nc r="Q82" t="inlineStr">
-      <is>
-        <t>ta</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
+  <rcc rId="1448" sId="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_diamondng.py  --synthesis=lse  --run-par-trce</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>cmd = python DEV/bin/run_diamondng.py  --synthesis=lse  --run-par-iota</t>
+        <phoneticPr fontId="0" type="noConversion"/>
       </is>
     </nc>
   </rcc>
@@ -5452,136 +6171,12 @@
 
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1334" sId="2">
-    <nc r="A83" t="inlineStr">
-      <is>
-        <t>81</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1335" sId="2">
-    <nc r="A84" t="inlineStr">
-      <is>
-        <t>82</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
   <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>case!$A$2:$AB$2</formula>
     <oldFormula>case!$A$2:$AB$2</oldFormula>
   </rdn>
   <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1337" sId="2">
-    <nc r="D83" t="inlineStr">
-      <is>
-        <t>set_false_path</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1338" sId="2">
-    <nc r="E83" t="inlineStr">
-      <is>
-        <t>SDC_cases/10_set_false_path/through_cells_04</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1339" sId="2">
-    <nc r="D84" t="inlineStr">
-      <is>
-        <t>create_generated_clock</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1340" sId="2">
-    <nc r="E84" t="inlineStr">
-      <is>
-        <t>SDC_cases/02_create_generated_clock/edges_nets_01</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1341" sId="2">
-    <nc r="Q83" t="inlineStr">
-      <is>
-        <t>ta</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="1342" sId="2">
-    <nc r="Q84" t="inlineStr">
-      <is>
-        <t>ta</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>case!$A$2:$AB$2</formula>
-    <oldFormula>case!$A$2:$AB$2</oldFormula>
-  </rdn>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>case!$A$2:$AB$2</formula>
-    <oldFormula>case!$A$2:$AB$2</oldFormula>
-  </rdn>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1345" sId="2" xfDxf="1" dxf="1">
-    <oc r="E83" t="inlineStr">
-      <is>
-        <t>SDC_cases/10_set_false_path/through_cells_04</t>
-      </is>
-    </oc>
-    <nc r="E83" t="inlineStr">
-      <is>
-        <t>SDC_cases/10_set_false_path/from_clk_01</t>
-      </is>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0"/>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1346" sId="2" xfDxf="1" dxf="1">
-    <oc r="E83" t="inlineStr">
-      <is>
-        <t>SDC_cases/10_set_false_path/from_clk_01</t>
-      </is>
-    </oc>
-    <nc r="E83" t="inlineStr">
-      <is>
-        <t>SDC_cases/10_set_false_path/to_cells_01</t>
-      </is>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0"/>
-    </ndxf>
-  </rcc>
 </revisions>
 </file>
 
@@ -5900,7 +6495,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5929,7 +6524,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5937,12 +6532,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5955,7 +6550,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>250</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5963,7 +6558,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5984,8 +6579,8 @@
   </sheetData>
   <sheetProtection password="DD9F" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5994,7 +6589,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -6007,14 +6603,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB84"/>
+  <dimension ref="A1:AB88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6166,30 +6762,36 @@
     </row>
     <row r="3" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>253</v>
+      <c r="M3" s="18" t="s">
+        <v>431</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -6197,13 +6799,16 @@
         <v>246</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -6211,13 +6816,16 @@
         <v>243</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -6225,13 +6833,16 @@
         <v>247</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -6239,41 +6850,50 @@
         <v>245</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -6281,1047 +6901,1316 @@
         <v>249</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q13" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q16" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q17" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q18" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q20" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q21" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q22" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q23" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q24" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D25" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>276</v>
+      <c r="M25" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q25" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q26" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q27" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q28" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
+      </c>
+      <c r="M29" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q29" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="M30" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q30" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
+      </c>
+      <c r="M31" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q31" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
+      </c>
+      <c r="M32" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q32" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
+      </c>
+      <c r="M33" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
+      </c>
+      <c r="M34" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q34" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+      <c r="M35" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q35" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q36" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q37" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q38" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q39" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="M40" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q40" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q41" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q42" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="M43" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q43" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="M44" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q44" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="M45" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q45" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="M46" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q46" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D47" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="E47" s="18" t="s">
-        <v>299</v>
+      <c r="M47" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q47" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q48" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
+      </c>
+      <c r="M49" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q49" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="M50" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q50" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
+      </c>
+      <c r="M51" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q51" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="M52" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q52" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
+      </c>
+      <c r="M53" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q53" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
+      </c>
+      <c r="M54" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q54" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
+      </c>
+      <c r="M55" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q55" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
+      </c>
+      <c r="M56" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q56" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="M57" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q57" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
+      </c>
+      <c r="M58" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q58" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
+      </c>
+      <c r="M59" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q59" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
+      </c>
+      <c r="M60" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q60" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="M61" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q61" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="M62" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q62" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="M63" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q63" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
+      </c>
+      <c r="M64" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q64" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
+      </c>
+      <c r="M65" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q65" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="M66" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q66" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
+      </c>
+      <c r="M67" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q67" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
+      </c>
+      <c r="M68" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q68" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D69" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E69" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="E69" s="18" t="s">
-        <v>322</v>
+      <c r="M69" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q69" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
+      </c>
+      <c r="M70" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q70" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
+      </c>
+      <c r="M71" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q71" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
+      </c>
+      <c r="M72" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q72" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
+      </c>
+      <c r="M73" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q73" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
+      </c>
+      <c r="M74" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q74" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
+      </c>
+      <c r="M75" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q75" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
+      </c>
+      <c r="M76" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q76" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
+      </c>
+      <c r="M77" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q77" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
+      </c>
+      <c r="M78" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q78" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="M79" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q79" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
+      </c>
+      <c r="M80" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q80" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="M81" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q81" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="M82" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q82" s="18" t="s">
         <v>413</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="E82" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q82" s="18" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
+      </c>
+      <c r="M83" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q83" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>419</v>
+        <v>421</v>
+      </c>
+      <c r="M84" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="Q84" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="M85" s="18" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="DD9F" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AB2"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AB2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -7330,12 +8219,12 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AB2"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -7459,17 +8348,17 @@
       <c r="E109" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F109" s="68" t="s">
+      <c r="F109" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="G109" s="69"/>
-      <c r="H109" s="69"/>
-      <c r="I109" s="69"/>
-      <c r="J109" s="69"/>
-      <c r="K109" s="69"/>
-      <c r="L109" s="69"/>
-      <c r="M109" s="69"/>
-      <c r="N109" s="70"/>
+      <c r="G109" s="54"/>
+      <c r="H109" s="54"/>
+      <c r="I109" s="54"/>
+      <c r="J109" s="54"/>
+      <c r="K109" s="54"/>
+      <c r="L109" s="54"/>
+      <c r="M109" s="54"/>
+      <c r="N109" s="55"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
@@ -8249,7 +9138,7 @@
       <c r="A142" s="41">
         <v>1</v>
       </c>
-      <c r="B142" s="71" t="s">
+      <c r="B142" s="56" t="s">
         <v>125</v>
       </c>
       <c r="C142" s="39" t="s">
@@ -8275,7 +9164,7 @@
       <c r="A143" s="41">
         <v>2</v>
       </c>
-      <c r="B143" s="72"/>
+      <c r="B143" s="57"/>
       <c r="C143" s="39" t="s">
         <v>131</v>
       </c>
@@ -8297,7 +9186,7 @@
       <c r="A144" s="41">
         <v>3</v>
       </c>
-      <c r="B144" s="72"/>
+      <c r="B144" s="57"/>
       <c r="C144" s="39" t="s">
         <v>9</v>
       </c>
@@ -8315,7 +9204,7 @@
       <c r="A145" s="41">
         <v>4</v>
       </c>
-      <c r="B145" s="72"/>
+      <c r="B145" s="57"/>
       <c r="C145" s="39" t="s">
         <v>39</v>
       </c>
@@ -8335,7 +9224,7 @@
       <c r="A146" s="41">
         <v>5</v>
       </c>
-      <c r="B146" s="72"/>
+      <c r="B146" s="57"/>
       <c r="C146" s="39" t="s">
         <v>133</v>
       </c>
@@ -8357,7 +9246,7 @@
       <c r="A147" s="41">
         <v>6</v>
       </c>
-      <c r="B147" s="72"/>
+      <c r="B147" s="57"/>
       <c r="C147" s="39" t="s">
         <v>42</v>
       </c>
@@ -8379,7 +9268,7 @@
       <c r="A148" s="41">
         <v>7</v>
       </c>
-      <c r="B148" s="72"/>
+      <c r="B148" s="57"/>
       <c r="C148" s="39" t="s">
         <v>57</v>
       </c>
@@ -8473,7 +9362,7 @@
       <c r="A152" s="41">
         <v>11</v>
       </c>
-      <c r="B152" s="71" t="s">
+      <c r="B152" s="56" t="s">
         <v>147</v>
       </c>
       <c r="C152" s="39" t="s">
@@ -8807,7 +9696,7 @@
       <c r="A168" s="42">
         <v>27</v>
       </c>
-      <c r="B168" s="53"/>
+      <c r="B168" s="59"/>
       <c r="C168" s="40"/>
       <c r="D168" s="40"/>
       <c r="E168" s="40"/>
@@ -8838,11 +9727,11 @@
       <c r="B181" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C181" s="64" t="s">
+      <c r="C181" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="D181" s="64"/>
-      <c r="E181" s="64"/>
+      <c r="D181" s="60"/>
+      <c r="E181" s="60"/>
       <c r="F181" s="34" t="s">
         <v>44</v>
       </c>
@@ -8857,11 +9746,11 @@
       <c r="B182" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="C182" s="65" t="s">
+      <c r="C182" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="D182" s="65"/>
-      <c r="E182" s="65"/>
+      <c r="D182" s="61"/>
+      <c r="E182" s="61"/>
       <c r="F182" s="39" t="s">
         <v>188</v>
       </c>
@@ -8872,11 +9761,11 @@
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="52"/>
       <c r="B183" s="52"/>
-      <c r="C183" s="66" t="s">
+      <c r="C183" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="D183" s="66"/>
-      <c r="E183" s="66"/>
+      <c r="D183" s="62"/>
+      <c r="E183" s="62"/>
       <c r="F183" s="39" t="s">
         <v>190</v>
       </c>
@@ -8889,11 +9778,11 @@
       <c r="B184" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="C184" s="67" t="s">
+      <c r="C184" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="D184" s="67"/>
-      <c r="E184" s="67"/>
+      <c r="D184" s="63"/>
+      <c r="E184" s="63"/>
       <c r="F184" s="39" t="s">
         <v>188</v>
       </c>
@@ -8904,11 +9793,11 @@
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="52"/>
       <c r="B185" s="52"/>
-      <c r="C185" s="67" t="s">
+      <c r="C185" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="D185" s="67"/>
-      <c r="E185" s="67"/>
+      <c r="D185" s="63"/>
+      <c r="E185" s="63"/>
       <c r="F185" s="39" t="s">
         <v>190</v>
       </c>
@@ -8917,7 +9806,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="54" t="s">
+      <c r="A186" s="64" t="s">
         <v>193</v>
       </c>
       <c r="B186" s="52" t="s">
@@ -8936,7 +9825,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="54"/>
+      <c r="A187" s="64"/>
       <c r="B187" s="52"/>
       <c r="C187" s="52" t="s">
         <v>47</v>
@@ -8951,7 +9840,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="54"/>
+      <c r="A188" s="64"/>
       <c r="B188" s="52" t="s">
         <v>195</v>
       </c>
@@ -8968,7 +9857,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" s="54"/>
+      <c r="A189" s="64"/>
       <c r="B189" s="52"/>
       <c r="C189" s="52" t="s">
         <v>49</v>
@@ -8983,7 +9872,7 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" s="54" t="s">
+      <c r="A190" s="64" t="s">
         <v>196</v>
       </c>
       <c r="B190" s="52" t="s">
@@ -9002,7 +9891,7 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" s="54"/>
+      <c r="A191" s="64"/>
       <c r="B191" s="52"/>
       <c r="C191" s="52" t="s">
         <v>51</v>
@@ -9017,7 +9906,7 @@
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="54"/>
+      <c r="A192" s="64"/>
       <c r="B192" s="52" t="s">
         <v>198</v>
       </c>
@@ -9034,13 +9923,13 @@
       </c>
     </row>
     <row r="193" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="55"/>
-      <c r="B193" s="53"/>
-      <c r="C193" s="53" t="s">
+      <c r="A193" s="65"/>
+      <c r="B193" s="59"/>
+      <c r="C193" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="D193" s="53"/>
-      <c r="E193" s="53"/>
+      <c r="D193" s="59"/>
+      <c r="E193" s="59"/>
       <c r="F193" s="40" t="s">
         <v>190</v>
       </c>
@@ -9079,12 +9968,12 @@
       <c r="A198" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="B198" s="56" t="s">
+      <c r="B198" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="C198" s="56"/>
-      <c r="D198" s="56"/>
-      <c r="E198" s="56"/>
+      <c r="C198" s="66"/>
+      <c r="D198" s="66"/>
+      <c r="E198" s="66"/>
       <c r="F198" s="22" t="s">
         <v>204</v>
       </c>
@@ -9096,7 +9985,7 @@
       <c r="A199" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="B199" s="57" t="s">
+      <c r="B199" s="67" t="s">
         <v>207</v>
       </c>
       <c r="C199" s="58"/>
@@ -9113,12 +10002,12 @@
       <c r="A200" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B200" s="59" t="s">
+      <c r="B200" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="C200" s="60"/>
-      <c r="D200" s="60"/>
-      <c r="E200" s="61"/>
+      <c r="C200" s="69"/>
+      <c r="D200" s="69"/>
+      <c r="E200" s="70"/>
       <c r="F200" s="10" t="s">
         <v>189</v>
       </c>
@@ -9130,12 +10019,12 @@
       <c r="A201" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="B201" s="59" t="s">
+      <c r="B201" s="68" t="s">
         <v>240</v>
       </c>
-      <c r="C201" s="60"/>
-      <c r="D201" s="60"/>
-      <c r="E201" s="61"/>
+      <c r="C201" s="69"/>
+      <c r="D201" s="69"/>
+      <c r="E201" s="70"/>
       <c r="F201" s="46" t="s">
         <v>238</v>
       </c>
@@ -9147,12 +10036,12 @@
       <c r="A202" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="B202" s="62" t="s">
+      <c r="B202" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="C202" s="53"/>
-      <c r="D202" s="53"/>
-      <c r="E202" s="53"/>
+      <c r="C202" s="59"/>
+      <c r="D202" s="59"/>
+      <c r="E202" s="59"/>
       <c r="F202" s="13" t="s">
         <v>189</v>
       </c>
@@ -9197,11 +10086,11 @@
       <c r="C207" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D207" s="63" t="s">
+      <c r="D207" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="E207" s="63"/>
-      <c r="F207" s="63"/>
+      <c r="E207" s="72"/>
+      <c r="F207" s="72"/>
       <c r="G207" s="32"/>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -9293,9 +10182,9 @@
       <c r="A213" s="42"/>
       <c r="B213" s="40"/>
       <c r="C213" s="40"/>
-      <c r="D213" s="53"/>
-      <c r="E213" s="53"/>
-      <c r="F213" s="53"/>
+      <c r="D213" s="59"/>
+      <c r="E213" s="59"/>
+      <c r="F213" s="59"/>
       <c r="G213" s="25"/>
     </row>
   </sheetData>
@@ -9307,28 +10196,11 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="41">
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="F109:N109"/>
-    <mergeCell ref="B142:B149"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="B154:B161"/>
-    <mergeCell ref="B165:B168"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="D209:F209"/>
+    <mergeCell ref="D210:F210"/>
+    <mergeCell ref="D211:F211"/>
+    <mergeCell ref="D212:F212"/>
+    <mergeCell ref="D213:F213"/>
     <mergeCell ref="D208:F208"/>
     <mergeCell ref="A190:A193"/>
     <mergeCell ref="B190:B191"/>
@@ -9343,11 +10215,28 @@
     <mergeCell ref="B202:E202"/>
     <mergeCell ref="D207:F207"/>
     <mergeCell ref="B201:E201"/>
-    <mergeCell ref="D209:F209"/>
-    <mergeCell ref="D210:F210"/>
-    <mergeCell ref="D211:F211"/>
-    <mergeCell ref="D212:F212"/>
-    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="B165:B168"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="B142:B149"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="B154:B161"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9371,15 +10260,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i230--EIT2 ta and mpar suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/analysis_00_ta_engine_all.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/analysis_00_ta_engine_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\test\analysis_00_ta_engine\hold_correction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repository\tmp_client\doc\TMP_EIT_suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="DD9F" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="6300" windowWidth="28836" windowHeight="6240"/>
+    <workbookView xWindow="-12" yWindow="6300" windowWidth="28836" windowHeight="6240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="426">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1482,26 +1482,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>set_clock_uncertainty</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>80</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ta</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>81</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>82</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>set_false_path</t>
   </si>
   <si>
@@ -1531,27 +1515,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>83</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold correction</t>
-  </si>
-  <si>
-    <t>hold correction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold correction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
     <t>cmd = --devkit=iCE40UP5K-CM225I</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1560,24 +1523,17 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>84</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold_correction/hold_correction1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold_correction/hold_correction2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold_correction/hold_correction3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>cmd = python DEV/bin/run_diamondng.py  --synthesis=lse  --run-par-iota</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
   </si>
 </sst>
 </file>
@@ -5243,7 +5199,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{655D6220-6132-41C2-8290-FCF487860342}" diskRevisions="1" revisionId="1450" version="35">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B6D1F743-3429-4AAD-B4BB-92240E62B112}" diskRevisions="1" revisionId="1459" version="38">
   <header guid="{962A471B-F009-4B00-939D-E8F2DC59916E}" dateTime="2018-10-12T14:54:08" maxSheetId="5" userName="Jason Wang" r:id="rId29" minRId="1347">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5300,6 +5256,30 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{9BF4050C-1AC4-4952-914D-5524D657763D}" dateTime="2019-10-23T14:41:40" maxSheetId="5" userName="Jason Wang" r:id="rId36" minRId="1451" maxRId="1453">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{482B65FE-E91A-4D0E-B478-3261A88F5FD1}" dateTime="2019-10-23T14:42:00" maxSheetId="5" userName="Jason Wang" r:id="rId37" minRId="1454">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B6D1F743-3429-4AAD-B4BB-92240E62B112}" dateTime="2019-10-23T14:56:04" maxSheetId="5" userName="Jason Wang" r:id="rId38" minRId="1455" maxRId="1458">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -6180,26 +6160,234 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1347" sId="1">
-    <oc r="B3" t="inlineStr">
-      <is>
-        <t>analysis_00_ta_engine</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
-      </is>
-    </oc>
-    <nc r="B3" t="inlineStr">
-      <is>
-        <t>T+_analysis_00_ta_engine</t>
-        <phoneticPr fontId="50049" type="noConversion"/>
+  <rrc rId="1451" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>84</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>hold correction</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>hold_correction/hold_correction1</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="1452" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>hold correction</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>hold_correction/hold_correction2</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="1453" sId="2" ref="A86:XFD86" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A86:XFD86" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A86" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D86" t="inlineStr">
+        <is>
+          <t>hold correction</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E86" t="inlineStr">
+        <is>
+          <t>hold_correction/hold_correction3</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1454" sId="2">
+    <nc r="Q85" t="inlineStr">
+      <is>
+        <t>ta</t>
+        <phoneticPr fontId="0" type="noConversion"/>
       </is>
     </nc>
   </rcc>
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1455" sId="2" ref="A82:XFD82" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A82:XFD82" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A82" t="inlineStr">
+        <is>
+          <t>80</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D82" t="inlineStr">
+        <is>
+          <t>set_clock_uncertainty</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E82" t="inlineStr">
+        <is>
+          <t>SDC_cases/04_set_clock_uncertainty/from_to_02</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="M82" t="inlineStr">
+        <is>
+          <t>cmd = --devkit=iCE40UP5K-CM225I</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="Q82" t="inlineStr">
+        <is>
+          <t>ta</t>
+          <phoneticPr fontId="0" type="noConversion"/>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="1456" sId="2">
+    <oc r="A82" t="inlineStr">
+      <is>
+        <t>81</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1457" sId="2">
+    <oc r="A83" t="inlineStr">
+      <is>
+        <t>82</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1458" sId="2">
+    <oc r="A84" t="inlineStr">
+      <is>
+        <t>83</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AB$2</formula>
+    <oldFormula>case!$A$2:$AB$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1347" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>analysis_00_ta_engine</t>
+        <phoneticPr fontId="50049" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>T+_analysis_00_ta_engine</t>
+        <phoneticPr fontId="50049" type="noConversion"/>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{962A471B-F009-4B00-939D-E8F2DC59916E}" name="Jason Wang" id="-981787801" dateTime="2018-10-12T15:16:31"/>
 </users>
@@ -6494,8 +6682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6524,7 +6712,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6550,7 +6738,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6558,7 +6746,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6603,14 +6791,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB88"/>
+  <dimension ref="A1:AB84"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomRight" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6771,7 +6959,7 @@
         <v>252</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="Q3" s="18" t="s">
         <v>408</v>
@@ -6788,7 +6976,7 @@
         <v>253</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q4" s="18" t="s">
         <v>409</v>
@@ -6805,7 +6993,7 @@
         <v>254</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q5" s="18" t="s">
         <v>409</v>
@@ -6822,7 +7010,7 @@
         <v>255</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q6" s="18" t="s">
         <v>408</v>
@@ -6839,7 +7027,7 @@
         <v>256</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q7" s="18" t="s">
         <v>409</v>
@@ -6856,7 +7044,7 @@
         <v>257</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q8" s="18" t="s">
         <v>408</v>
@@ -6873,7 +7061,7 @@
         <v>258</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q9" s="18" t="s">
         <v>409</v>
@@ -6890,7 +7078,7 @@
         <v>259</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q10" s="18" t="s">
         <v>408</v>
@@ -6907,7 +7095,7 @@
         <v>260</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q11" s="18" t="s">
         <v>409</v>
@@ -6924,7 +7112,7 @@
         <v>261</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q12" s="18" t="s">
         <v>408</v>
@@ -6941,7 +7129,7 @@
         <v>262</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q13" s="18" t="s">
         <v>409</v>
@@ -6958,7 +7146,7 @@
         <v>263</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q14" s="18" t="s">
         <v>408</v>
@@ -6975,7 +7163,7 @@
         <v>264</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q15" s="18" t="s">
         <v>409</v>
@@ -6992,7 +7180,7 @@
         <v>265</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q16" s="18" t="s">
         <v>408</v>
@@ -7009,7 +7197,7 @@
         <v>266</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q17" s="18" t="s">
         <v>409</v>
@@ -7026,7 +7214,7 @@
         <v>267</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q18" s="18" t="s">
         <v>408</v>
@@ -7043,7 +7231,7 @@
         <v>268</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q19" s="18" t="s">
         <v>409</v>
@@ -7060,7 +7248,7 @@
         <v>269</v>
       </c>
       <c r="M20" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q20" s="18" t="s">
         <v>408</v>
@@ -7077,7 +7265,7 @@
         <v>270</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q21" s="18" t="s">
         <v>409</v>
@@ -7094,7 +7282,7 @@
         <v>271</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q22" s="18" t="s">
         <v>408</v>
@@ -7111,7 +7299,7 @@
         <v>272</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q23" s="18" t="s">
         <v>409</v>
@@ -7128,7 +7316,7 @@
         <v>273</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q24" s="18" t="s">
         <v>408</v>
@@ -7145,7 +7333,7 @@
         <v>275</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q25" s="18" t="s">
         <v>409</v>
@@ -7162,7 +7350,7 @@
         <v>276</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q26" s="18" t="s">
         <v>408</v>
@@ -7179,7 +7367,7 @@
         <v>277</v>
       </c>
       <c r="M27" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q27" s="18" t="s">
         <v>409</v>
@@ -7196,7 +7384,7 @@
         <v>278</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q28" s="18" t="s">
         <v>408</v>
@@ -7213,7 +7401,7 @@
         <v>279</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q29" s="18" t="s">
         <v>409</v>
@@ -7230,7 +7418,7 @@
         <v>280</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q30" s="18" t="s">
         <v>408</v>
@@ -7247,7 +7435,7 @@
         <v>281</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q31" s="18" t="s">
         <v>409</v>
@@ -7264,7 +7452,7 @@
         <v>282</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q32" s="18" t="s">
         <v>408</v>
@@ -7281,7 +7469,7 @@
         <v>283</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q33" s="18" t="s">
         <v>409</v>
@@ -7298,7 +7486,7 @@
         <v>284</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q34" s="18" t="s">
         <v>408</v>
@@ -7315,7 +7503,7 @@
         <v>285</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q35" s="18" t="s">
         <v>409</v>
@@ -7332,7 +7520,7 @@
         <v>286</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q36" s="18" t="s">
         <v>408</v>
@@ -7349,7 +7537,7 @@
         <v>287</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q37" s="18" t="s">
         <v>409</v>
@@ -7366,7 +7554,7 @@
         <v>288</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q38" s="18" t="s">
         <v>408</v>
@@ -7383,7 +7571,7 @@
         <v>289</v>
       </c>
       <c r="M39" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q39" s="18" t="s">
         <v>409</v>
@@ -7400,7 +7588,7 @@
         <v>290</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q40" s="18" t="s">
         <v>408</v>
@@ -7417,7 +7605,7 @@
         <v>291</v>
       </c>
       <c r="M41" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q41" s="18" t="s">
         <v>409</v>
@@ -7434,7 +7622,7 @@
         <v>292</v>
       </c>
       <c r="M42" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q42" s="18" t="s">
         <v>408</v>
@@ -7451,7 +7639,7 @@
         <v>293</v>
       </c>
       <c r="M43" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q43" s="18" t="s">
         <v>409</v>
@@ -7468,7 +7656,7 @@
         <v>294</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q44" s="18" t="s">
         <v>408</v>
@@ -7485,7 +7673,7 @@
         <v>295</v>
       </c>
       <c r="M45" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q45" s="18" t="s">
         <v>409</v>
@@ -7502,7 +7690,7 @@
         <v>296</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q46" s="18" t="s">
         <v>408</v>
@@ -7519,7 +7707,7 @@
         <v>298</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q47" s="18" t="s">
         <v>409</v>
@@ -7536,7 +7724,7 @@
         <v>299</v>
       </c>
       <c r="M48" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q48" s="18" t="s">
         <v>408</v>
@@ -7553,7 +7741,7 @@
         <v>300</v>
       </c>
       <c r="M49" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q49" s="18" t="s">
         <v>409</v>
@@ -7570,7 +7758,7 @@
         <v>301</v>
       </c>
       <c r="M50" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q50" s="18" t="s">
         <v>408</v>
@@ -7587,7 +7775,7 @@
         <v>302</v>
       </c>
       <c r="M51" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q51" s="18" t="s">
         <v>409</v>
@@ -7604,7 +7792,7 @@
         <v>303</v>
       </c>
       <c r="M52" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q52" s="18" t="s">
         <v>408</v>
@@ -7621,7 +7809,7 @@
         <v>304</v>
       </c>
       <c r="M53" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q53" s="18" t="s">
         <v>409</v>
@@ -7638,7 +7826,7 @@
         <v>305</v>
       </c>
       <c r="M54" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q54" s="18" t="s">
         <v>408</v>
@@ -7655,7 +7843,7 @@
         <v>306</v>
       </c>
       <c r="M55" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q55" s="18" t="s">
         <v>409</v>
@@ -7672,7 +7860,7 @@
         <v>307</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q56" s="18" t="s">
         <v>408</v>
@@ -7689,7 +7877,7 @@
         <v>308</v>
       </c>
       <c r="M57" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q57" s="18" t="s">
         <v>409</v>
@@ -7706,7 +7894,7 @@
         <v>309</v>
       </c>
       <c r="M58" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q58" s="18" t="s">
         <v>408</v>
@@ -7723,7 +7911,7 @@
         <v>310</v>
       </c>
       <c r="M59" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q59" s="18" t="s">
         <v>409</v>
@@ -7740,7 +7928,7 @@
         <v>311</v>
       </c>
       <c r="M60" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q60" s="18" t="s">
         <v>408</v>
@@ -7757,7 +7945,7 @@
         <v>312</v>
       </c>
       <c r="M61" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q61" s="18" t="s">
         <v>409</v>
@@ -7774,7 +7962,7 @@
         <v>313</v>
       </c>
       <c r="M62" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q62" s="18" t="s">
         <v>408</v>
@@ -7791,7 +7979,7 @@
         <v>314</v>
       </c>
       <c r="M63" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q63" s="18" t="s">
         <v>409</v>
@@ -7808,7 +7996,7 @@
         <v>315</v>
       </c>
       <c r="M64" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q64" s="18" t="s">
         <v>408</v>
@@ -7825,7 +8013,7 @@
         <v>316</v>
       </c>
       <c r="M65" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q65" s="18" t="s">
         <v>409</v>
@@ -7842,7 +8030,7 @@
         <v>317</v>
       </c>
       <c r="M66" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q66" s="18" t="s">
         <v>408</v>
@@ -7859,7 +8047,7 @@
         <v>318</v>
       </c>
       <c r="M67" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q67" s="18" t="s">
         <v>409</v>
@@ -7876,7 +8064,7 @@
         <v>319</v>
       </c>
       <c r="M68" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q68" s="18" t="s">
         <v>408</v>
@@ -7893,7 +8081,7 @@
         <v>321</v>
       </c>
       <c r="M69" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q69" s="18" t="s">
         <v>409</v>
@@ -7910,7 +8098,7 @@
         <v>322</v>
       </c>
       <c r="M70" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q70" s="18" t="s">
         <v>408</v>
@@ -7927,7 +8115,7 @@
         <v>323</v>
       </c>
       <c r="M71" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q71" s="18" t="s">
         <v>409</v>
@@ -7944,7 +8132,7 @@
         <v>324</v>
       </c>
       <c r="M72" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q72" s="18" t="s">
         <v>408</v>
@@ -7961,7 +8149,7 @@
         <v>325</v>
       </c>
       <c r="M73" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q73" s="18" t="s">
         <v>409</v>
@@ -7978,7 +8166,7 @@
         <v>326</v>
       </c>
       <c r="M74" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q74" s="18" t="s">
         <v>408</v>
@@ -7995,7 +8183,7 @@
         <v>327</v>
       </c>
       <c r="M75" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q75" s="18" t="s">
         <v>409</v>
@@ -8012,7 +8200,7 @@
         <v>328</v>
       </c>
       <c r="M76" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q76" s="18" t="s">
         <v>408</v>
@@ -8029,7 +8217,7 @@
         <v>329</v>
       </c>
       <c r="M77" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q77" s="18" t="s">
         <v>409</v>
@@ -8046,7 +8234,7 @@
         <v>330</v>
       </c>
       <c r="M78" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q78" s="18" t="s">
         <v>408</v>
@@ -8063,7 +8251,7 @@
         <v>331</v>
       </c>
       <c r="M79" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q79" s="18" t="s">
         <v>409</v>
@@ -8080,7 +8268,7 @@
         <v>332</v>
       </c>
       <c r="M80" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q80" s="18" t="s">
         <v>408</v>
@@ -8097,7 +8285,7 @@
         <v>333</v>
       </c>
       <c r="M81" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q81" s="18" t="s">
         <v>409</v>
@@ -8105,100 +8293,53 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="D82" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="E82" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="M82" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q82" s="18" t="s">
         <v>411</v>
-      </c>
-      <c r="E82" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="M82" s="18" t="s">
-        <v>430</v>
-      </c>
-      <c r="Q82" s="18" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M83" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q83" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="M84" s="18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="Q84" s="18" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="M85" s="18" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="D86" s="18" t="s">
-        <v>426</v>
-      </c>
-      <c r="E86" s="18" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
-        <v>428</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>425</v>
-      </c>
-      <c r="E87" s="18" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>427</v>
-      </c>
-      <c r="E88" s="18" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -8206,8 +8347,8 @@
   <autoFilter ref="A2:AB2"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B88" sqref="B88"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A2:AB2"/>
@@ -8244,6 +8385,12 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>description!$F$118:$J$118</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:T1 J1:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>description!$F$129:$G$129</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
@@ -8271,12 +8418,6 @@
             <xm:f>description!$F$136:$H$136</xm:f>
           </x14:formula1>
           <xm:sqref>AA1:AA1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>description!$F$118:$J$118</xm:f>
-          </x14:formula1>
-          <xm:sqref>J1:J1048576 A1:T1 J2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>